<commit_message>
Fixed point iteration 2 and 3
</commit_message>
<xml_diff>
--- a/FINAL_FILES/sweeping_fractional_bit_widths_for_weights_biases_slope_parameters.xlsx
+++ b/FINAL_FILES/sweeping_fractional_bit_widths_for_weights_biases_slope_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEW\Desktop\DVLSI_ML_Project\FINAL_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECBB4C9-F077-4177-8568-F38AFE91AED5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76FC4CF-EEED-4B18-89D0-1E82944DD7F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{505DE35A-2780-41A3-A4D9-27FC10F55B2C}"/>
   </bookViews>
@@ -57,19 +57,19 @@
     <t>slope in Leaky ReLU</t>
   </si>
   <si>
-    <t>Chosen representation for w12: Q2.13</t>
-  </si>
-  <si>
-    <t>Chosen representation for b12: Q3.13</t>
-  </si>
-  <si>
-    <t>Chosen representation for b23: Q2.12</t>
-  </si>
-  <si>
     <t>Chosen representation for slope: Q2.12</t>
   </si>
   <si>
-    <t>Chosen representation for w23: Q2.12</t>
+    <t>Chosen representation for w12: Q10.8</t>
+  </si>
+  <si>
+    <t>Chosen representation for w23: Q10.8</t>
+  </si>
+  <si>
+    <t>Chosen representation for b12: Q15.12</t>
+  </si>
+  <si>
+    <t>Chosen representation for b23: Q13.11</t>
   </si>
 </sst>
 </file>
@@ -6585,8 +6585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78AF8B31-42CA-4C26-92F8-C111DC46B288}">
   <dimension ref="B2:L190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77:L77"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O148" sqref="O148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6875,7 +6875,7 @@
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H38" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -7161,7 +7161,7 @@
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H77" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
@@ -7447,7 +7447,7 @@
     </row>
     <row r="115" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H115" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
@@ -7733,7 +7733,7 @@
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H152" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I152" s="2"/>
       <c r="J152" s="2"/>
@@ -8019,7 +8019,7 @@
     </row>
     <row r="190" spans="4:12" x14ac:dyDescent="0.25">
       <c r="H190" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I190" s="2"/>
       <c r="J190" s="2"/>

</xml_diff>

<commit_message>
Created reference model, generated memory files, re-entering verilog phase
</commit_message>
<xml_diff>
--- a/FINAL_FILES/sweeping_fractional_bit_widths_for_weights_biases_slope_parameters.xlsx
+++ b/FINAL_FILES/sweeping_fractional_bit_widths_for_weights_biases_slope_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEW\Desktop\DVLSI_ML_Project\FINAL_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76FC4CF-EEED-4B18-89D0-1E82944DD7F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D297C347-3A58-4D12-8040-0BA8F0EC4A0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{505DE35A-2780-41A3-A4D9-27FC10F55B2C}"/>
   </bookViews>
@@ -6585,8 +6585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78AF8B31-42CA-4C26-92F8-C111DC46B288}">
   <dimension ref="B2:L190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O148" sqref="O148"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>